<commit_message>
Rename sheet for packaging #ST-785
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v2-packaging-msl.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v2-packaging-msl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="MSL Packaging" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Packaging" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -170,7 +170,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="15">
     <border/>
     <border>
       <left style="medium">
@@ -241,18 +241,7 @@
       <top/>
     </border>
     <border>
-      <right/>
       <top/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <bottom/>
-    </border>
-    <border>
-      <right/>
-      <bottom/>
     </border>
     <border>
       <left style="thin">
@@ -293,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -354,8 +343,7 @@
     <xf borderId="6" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
@@ -371,19 +359,19 @@
     <xf borderId="8" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="12" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="13" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="15" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="16" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -763,7 +751,6 @@
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
       <c r="F13" s="21"/>
@@ -782,39 +769,39 @@
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
-      <c r="H14" s="24"/>
+      <c r="H14" s="23"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="21"/>
-      <c r="B15" s="25"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
       <c r="G15" s="21"/>
-      <c r="H15" s="24"/>
+      <c r="H15" s="23"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="21"/>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="28" t="s">
+      <c r="H16" s="27" t="s">
         <v>21</v>
       </c>
     </row>
@@ -826,7 +813,7 @@
       <c r="C17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>24</v>
       </c>
       <c r="E17" s="10" t="s">
@@ -854,19 +841,19 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="14"/>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32" t="s">
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32" t="s">
+      <c r="F19" s="31"/>
+      <c r="G19" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="33"/>
+      <c r="H19" s="32"/>
     </row>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>

</xml_diff>